<commit_message>
New data and minor changes
</commit_message>
<xml_diff>
--- a/Raw Data/HUAWEI.xlsx
+++ b/Raw Data/HUAWEI.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="HUAWEI" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -349,7 +349,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D204"/>
+  <dimension ref="A1:D185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -374,2843 +374,2577 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43567</v>
+        <v>43586</v>
       </c>
       <c r="B2">
-        <v>3672</v>
+        <v>2104</v>
       </c>
       <c r="C2">
-        <v>2.78</v>
+        <v>1.59</v>
       </c>
       <c r="D2">
-        <v>119</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43568</v>
+        <v>43587</v>
       </c>
       <c r="B3">
-        <v>5223</v>
+        <v>5601</v>
       </c>
       <c r="C3">
-        <v>3.95</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="D3">
-        <v>170</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>43569</v>
+        <v>43588</v>
       </c>
       <c r="B4">
-        <v>1682</v>
+        <v>2921</v>
       </c>
       <c r="C4">
-        <v>1.27</v>
+        <v>2.21</v>
       </c>
       <c r="D4">
-        <v>55</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43570</v>
+        <v>43589</v>
       </c>
       <c r="B5">
-        <v>2713</v>
+        <v>2956</v>
       </c>
       <c r="C5">
-        <v>2.0499999999999998</v>
+        <v>2.23</v>
       </c>
       <c r="D5">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>43571</v>
+        <v>43590</v>
       </c>
       <c r="B6">
-        <v>16007</v>
+        <v>6337</v>
       </c>
       <c r="C6">
-        <v>12.1</v>
+        <v>4.79</v>
       </c>
       <c r="D6">
-        <v>545</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43572</v>
+        <v>43591</v>
       </c>
       <c r="B7">
-        <v>3164</v>
+        <v>5328</v>
       </c>
       <c r="C7">
-        <v>2.39</v>
+        <v>4.03</v>
       </c>
       <c r="D7">
-        <v>108</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43573</v>
+        <v>43592</v>
       </c>
       <c r="B8">
-        <v>10588</v>
+        <v>6679</v>
       </c>
       <c r="C8">
-        <v>8</v>
+        <v>5.0199999999999996</v>
       </c>
       <c r="D8">
-        <v>360</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43574</v>
+        <v>43593</v>
       </c>
       <c r="B9">
-        <v>2967</v>
+        <v>11008</v>
       </c>
       <c r="C9">
-        <v>2.2400000000000002</v>
+        <v>8.26</v>
       </c>
       <c r="D9">
-        <v>101</v>
+        <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43575</v>
+        <v>43594</v>
       </c>
       <c r="B10">
-        <v>8307</v>
+        <v>11218</v>
       </c>
       <c r="C10">
-        <v>6.28</v>
+        <v>8.48</v>
       </c>
       <c r="D10">
-        <v>283</v>
+        <v>382</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43576</v>
+        <v>43595</v>
       </c>
       <c r="B11">
-        <v>3754</v>
+        <v>11218</v>
       </c>
       <c r="C11">
-        <v>2.84</v>
+        <v>8.48</v>
       </c>
       <c r="D11">
-        <v>130</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43577</v>
+        <v>43596</v>
       </c>
       <c r="B12">
-        <v>9786</v>
+        <v>5134</v>
       </c>
       <c r="C12">
-        <v>7.4</v>
+        <v>3.88</v>
       </c>
       <c r="D12">
-        <v>333</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>43578</v>
+        <v>43597</v>
       </c>
       <c r="B13">
-        <v>8932</v>
+        <v>2522</v>
       </c>
       <c r="C13">
-        <v>6.75</v>
+        <v>1.91</v>
       </c>
       <c r="D13">
-        <v>304</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>43579</v>
+        <v>43598</v>
       </c>
       <c r="B14">
-        <v>4623</v>
+        <v>11166</v>
       </c>
       <c r="C14">
-        <v>3.49</v>
+        <v>8.44</v>
       </c>
       <c r="D14">
-        <v>157</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>43580</v>
+        <v>43599</v>
       </c>
       <c r="B15">
-        <v>3733</v>
+        <v>3139</v>
       </c>
       <c r="C15">
-        <v>2.82</v>
+        <v>2.37</v>
       </c>
       <c r="D15">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>43581</v>
+        <v>43600</v>
       </c>
       <c r="B16">
-        <v>6451</v>
+        <v>3703</v>
       </c>
       <c r="C16">
-        <v>4.88</v>
+        <v>2.8</v>
       </c>
       <c r="D16">
-        <v>221</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>43582</v>
+        <v>43601</v>
       </c>
       <c r="B17">
-        <v>2461</v>
+        <v>8870</v>
       </c>
       <c r="C17">
-        <v>1.86</v>
+        <v>6.71</v>
       </c>
       <c r="D17">
-        <v>84</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>43583</v>
+        <v>43602</v>
       </c>
       <c r="B18">
-        <v>4369</v>
+        <v>6275</v>
       </c>
       <c r="C18">
-        <v>3.3</v>
+        <v>4.74</v>
       </c>
       <c r="D18">
-        <v>149</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>43584</v>
+        <v>43603</v>
       </c>
       <c r="B19">
-        <v>5034</v>
+        <v>7253</v>
       </c>
       <c r="C19">
-        <v>3.81</v>
+        <v>5.48</v>
       </c>
       <c r="D19">
-        <v>171</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>43585</v>
+        <v>43604</v>
       </c>
       <c r="B20">
-        <v>6441</v>
+        <v>8722</v>
       </c>
       <c r="C20">
-        <v>4.87</v>
+        <v>6.59</v>
       </c>
       <c r="D20">
-        <v>223</v>
+        <v>297</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>43586</v>
+        <v>43605</v>
       </c>
       <c r="B21">
-        <v>2104</v>
+        <v>4378</v>
       </c>
       <c r="C21">
-        <v>1.59</v>
+        <v>3.31</v>
       </c>
       <c r="D21">
-        <v>72</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>43587</v>
+        <v>43606</v>
       </c>
       <c r="B22">
-        <v>5601</v>
+        <v>7665</v>
       </c>
       <c r="C22">
-        <v>4.2300000000000004</v>
+        <v>5.79</v>
       </c>
       <c r="D22">
-        <v>191</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>43588</v>
+        <v>43607</v>
       </c>
       <c r="B23">
-        <v>2921</v>
+        <v>6548</v>
       </c>
       <c r="C23">
-        <v>2.21</v>
+        <v>4.95</v>
       </c>
       <c r="D23">
-        <v>99</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>43589</v>
+        <v>43608</v>
       </c>
       <c r="B24">
-        <v>2956</v>
+        <v>4106</v>
       </c>
       <c r="C24">
-        <v>2.23</v>
+        <v>3.1</v>
       </c>
       <c r="D24">
-        <v>101</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>43590</v>
+        <v>43609</v>
       </c>
       <c r="B25">
-        <v>6337</v>
+        <v>5169</v>
       </c>
       <c r="C25">
-        <v>4.79</v>
+        <v>3.91</v>
       </c>
       <c r="D25">
-        <v>216</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>43591</v>
+        <v>43610</v>
       </c>
       <c r="B26">
-        <v>5328</v>
+        <v>3848</v>
       </c>
       <c r="C26">
-        <v>4.03</v>
+        <v>2.91</v>
       </c>
       <c r="D26">
-        <v>181</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>43592</v>
+        <v>43611</v>
       </c>
       <c r="B27">
-        <v>6679</v>
+        <v>9790</v>
       </c>
       <c r="C27">
-        <v>5.0199999999999996</v>
+        <v>7.4</v>
       </c>
       <c r="D27">
-        <v>226</v>
+        <v>333</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>43593</v>
+        <v>43612</v>
       </c>
       <c r="B28">
-        <v>11008</v>
+        <v>3290</v>
       </c>
       <c r="C28">
-        <v>8.26</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="D28">
-        <v>375</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>43594</v>
+        <v>43613</v>
       </c>
       <c r="B29">
-        <v>11218</v>
+        <v>2991</v>
       </c>
       <c r="C29">
-        <v>8.48</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="D29">
-        <v>382</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>43595</v>
+        <v>43614</v>
       </c>
       <c r="B30">
-        <v>11218</v>
+        <v>7767</v>
       </c>
       <c r="C30">
-        <v>8.48</v>
+        <v>5.87</v>
       </c>
       <c r="D30">
-        <v>382</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>43596</v>
+        <v>43615</v>
       </c>
       <c r="B31">
-        <v>5134</v>
+        <v>2915</v>
       </c>
       <c r="C31">
-        <v>3.88</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D31">
-        <v>175</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>43597</v>
+        <v>43616</v>
       </c>
       <c r="B32">
-        <v>2522</v>
+        <v>4951</v>
       </c>
       <c r="C32">
-        <v>1.91</v>
+        <v>3.74</v>
       </c>
       <c r="D32">
-        <v>86</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>43598</v>
+        <v>43617</v>
       </c>
       <c r="B33">
-        <v>11166</v>
+        <v>2439</v>
       </c>
       <c r="C33">
-        <v>8.44</v>
+        <v>1.84</v>
       </c>
       <c r="D33">
-        <v>380</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>43599</v>
+        <v>43618</v>
       </c>
       <c r="B34">
-        <v>3139</v>
+        <v>7282</v>
       </c>
       <c r="C34">
-        <v>2.37</v>
+        <v>5.51</v>
       </c>
       <c r="D34">
-        <v>107</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>43600</v>
+        <v>43619</v>
       </c>
       <c r="B35">
-        <v>3703</v>
+        <v>6725</v>
       </c>
       <c r="C35">
-        <v>2.8</v>
+        <v>5.08</v>
       </c>
       <c r="D35">
-        <v>126</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>43601</v>
+        <v>43620</v>
       </c>
       <c r="B36">
-        <v>8870</v>
+        <v>7750</v>
       </c>
       <c r="C36">
-        <v>6.71</v>
+        <v>5.86</v>
       </c>
       <c r="D36">
-        <v>302</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>43602</v>
+        <v>43621</v>
       </c>
       <c r="B37">
-        <v>6275</v>
+        <v>8031</v>
       </c>
       <c r="C37">
-        <v>4.74</v>
+        <v>6.07</v>
       </c>
       <c r="D37">
-        <v>216</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>43603</v>
+        <v>43622</v>
       </c>
       <c r="B38">
-        <v>7253</v>
+        <v>11105</v>
       </c>
       <c r="C38">
-        <v>5.48</v>
+        <v>8.4</v>
       </c>
       <c r="D38">
-        <v>247</v>
+        <v>378</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>43604</v>
+        <v>43623</v>
       </c>
       <c r="B39">
-        <v>8722</v>
+        <v>9018</v>
       </c>
       <c r="C39">
-        <v>6.59</v>
+        <v>6.81</v>
       </c>
       <c r="D39">
-        <v>297</v>
+        <v>306</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>43605</v>
+        <v>43624</v>
       </c>
       <c r="B40">
-        <v>4378</v>
+        <v>3241</v>
       </c>
       <c r="C40">
-        <v>3.31</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="D40">
-        <v>149</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>43606</v>
+        <v>43625</v>
       </c>
       <c r="B41">
-        <v>7665</v>
+        <v>3767</v>
       </c>
       <c r="C41">
-        <v>5.79</v>
+        <v>2.85</v>
       </c>
       <c r="D41">
-        <v>261</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>43607</v>
+        <v>43626</v>
       </c>
       <c r="B42">
-        <v>6548</v>
+        <v>5363</v>
       </c>
       <c r="C42">
-        <v>4.95</v>
+        <v>4.05</v>
       </c>
       <c r="D42">
-        <v>223</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>43608</v>
+        <v>43627</v>
       </c>
       <c r="B43">
-        <v>4106</v>
+        <v>18470</v>
       </c>
       <c r="C43">
-        <v>3.1</v>
+        <v>13.96</v>
       </c>
       <c r="D43">
-        <v>140</v>
+        <v>628</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>43609</v>
+        <v>43628</v>
       </c>
       <c r="B44">
-        <v>5169</v>
+        <v>4444</v>
       </c>
       <c r="C44">
-        <v>3.91</v>
+        <v>3.36</v>
       </c>
       <c r="D44">
-        <v>176</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>43610</v>
+        <v>43629</v>
       </c>
       <c r="B45">
-        <v>3848</v>
+        <v>9257</v>
       </c>
       <c r="C45">
-        <v>2.91</v>
+        <v>7</v>
       </c>
       <c r="D45">
-        <v>131</v>
+        <v>317</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>43611</v>
+        <v>43630</v>
       </c>
       <c r="B46">
-        <v>9790</v>
+        <v>13944</v>
       </c>
       <c r="C46">
-        <v>7.4</v>
+        <v>10.54</v>
       </c>
       <c r="D46">
-        <v>333</v>
+        <v>542</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>43612</v>
+        <v>43631</v>
       </c>
       <c r="B47">
-        <v>3290</v>
+        <v>11448</v>
       </c>
       <c r="C47">
-        <v>2.4900000000000002</v>
+        <v>8.65</v>
       </c>
       <c r="D47">
-        <v>112</v>
+        <v>389</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>43613</v>
+        <v>43632</v>
       </c>
       <c r="B48">
-        <v>2991</v>
+        <v>4732</v>
       </c>
       <c r="C48">
-        <v>2.2599999999999998</v>
+        <v>3.58</v>
       </c>
       <c r="D48">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>43614</v>
+        <v>43633</v>
       </c>
       <c r="B49">
-        <v>7767</v>
+        <v>4840</v>
       </c>
       <c r="C49">
-        <v>5.87</v>
+        <v>3.66</v>
       </c>
       <c r="D49">
-        <v>264</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>43615</v>
+        <v>43634</v>
       </c>
       <c r="B50">
-        <v>2915</v>
+        <v>14634</v>
       </c>
       <c r="C50">
-        <v>2.2000000000000002</v>
+        <v>11.06</v>
       </c>
       <c r="D50">
-        <v>99</v>
+        <v>498</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>43616</v>
+        <v>43635</v>
       </c>
       <c r="B51">
-        <v>4951</v>
+        <v>8074</v>
       </c>
       <c r="C51">
-        <v>3.74</v>
+        <v>6.1</v>
       </c>
       <c r="D51">
-        <v>168</v>
+        <v>383</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>43617</v>
+        <v>43636</v>
       </c>
       <c r="B52">
-        <v>2439</v>
+        <v>5392</v>
       </c>
       <c r="C52">
-        <v>1.84</v>
+        <v>4.08</v>
       </c>
       <c r="D52">
-        <v>83</v>
+        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>43618</v>
+        <v>43637</v>
       </c>
       <c r="B53">
-        <v>7282</v>
+        <v>13215</v>
       </c>
       <c r="C53">
-        <v>5.51</v>
+        <v>9.9</v>
       </c>
       <c r="D53">
-        <v>248</v>
+        <v>585</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>43619</v>
+        <v>43638</v>
       </c>
       <c r="B54">
-        <v>6725</v>
+        <v>4571</v>
       </c>
       <c r="C54">
-        <v>5.08</v>
+        <v>3.46</v>
       </c>
       <c r="D54">
-        <v>229</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>43620</v>
+        <v>43639</v>
       </c>
       <c r="B55">
-        <v>7750</v>
+        <v>481</v>
       </c>
       <c r="C55">
-        <v>5.86</v>
+        <v>0.36</v>
       </c>
       <c r="D55">
-        <v>264</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>43621</v>
+        <v>43640</v>
       </c>
       <c r="B56">
-        <v>8031</v>
+        <v>6663</v>
       </c>
       <c r="C56">
-        <v>6.07</v>
+        <v>5.04</v>
       </c>
       <c r="D56">
-        <v>273</v>
+        <v>367</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>43622</v>
+        <v>43641</v>
       </c>
       <c r="B57">
-        <v>11105</v>
+        <v>4203</v>
       </c>
       <c r="C57">
-        <v>8.4</v>
+        <v>3.18</v>
       </c>
       <c r="D57">
-        <v>378</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>43623</v>
+        <v>43642</v>
       </c>
       <c r="B58">
-        <v>9018</v>
+        <v>10404</v>
       </c>
       <c r="C58">
-        <v>6.81</v>
+        <v>7.87</v>
       </c>
       <c r="D58">
-        <v>306</v>
+        <v>355</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>43624</v>
+        <v>43643</v>
       </c>
       <c r="B59">
-        <v>3241</v>
+        <v>12662</v>
       </c>
       <c r="C59">
-        <v>2.4500000000000002</v>
+        <v>9.57</v>
       </c>
       <c r="D59">
-        <v>110</v>
+        <v>431</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>43625</v>
+        <v>43644</v>
       </c>
       <c r="B60">
-        <v>3767</v>
+        <v>7332</v>
       </c>
       <c r="C60">
-        <v>2.85</v>
+        <v>5.54</v>
       </c>
       <c r="D60">
-        <v>128</v>
+        <v>249</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>43626</v>
+        <v>43645</v>
       </c>
       <c r="B61">
-        <v>5363</v>
+        <v>6122</v>
       </c>
       <c r="C61">
-        <v>4.05</v>
+        <v>4.63</v>
       </c>
       <c r="D61">
-        <v>182</v>
+        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>43627</v>
+        <v>43646</v>
       </c>
       <c r="B62">
-        <v>18470</v>
+        <v>6625</v>
       </c>
       <c r="C62">
-        <v>13.96</v>
+        <v>5.01</v>
       </c>
       <c r="D62">
-        <v>628</v>
+        <v>225</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>43628</v>
+        <v>43647</v>
       </c>
       <c r="B63">
-        <v>4444</v>
+        <v>2296</v>
       </c>
       <c r="C63">
-        <v>3.36</v>
+        <v>1.74</v>
       </c>
       <c r="D63">
-        <v>151</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>43629</v>
+        <v>43648</v>
       </c>
       <c r="B64">
-        <v>9257</v>
+        <v>5171</v>
       </c>
       <c r="C64">
-        <v>7</v>
+        <v>3.91</v>
       </c>
       <c r="D64">
-        <v>317</v>
+        <v>176</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>43630</v>
+        <v>43649</v>
       </c>
       <c r="B65">
-        <v>13944</v>
+        <v>11882</v>
       </c>
       <c r="C65">
-        <v>10.54</v>
+        <v>8.98</v>
       </c>
       <c r="D65">
-        <v>542</v>
+        <v>404</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>43631</v>
+        <v>43650</v>
       </c>
       <c r="B66">
-        <v>11448</v>
+        <v>6006</v>
       </c>
       <c r="C66">
-        <v>8.65</v>
+        <v>4.54</v>
       </c>
       <c r="D66">
-        <v>389</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>43632</v>
+        <v>43651</v>
       </c>
       <c r="B67">
-        <v>4732</v>
+        <v>5774</v>
       </c>
       <c r="C67">
-        <v>3.58</v>
+        <v>4.37</v>
       </c>
       <c r="D67">
-        <v>161</v>
+        <v>196</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>43633</v>
+        <v>43652</v>
       </c>
       <c r="B68">
-        <v>4840</v>
+        <v>5344</v>
       </c>
       <c r="C68">
-        <v>3.66</v>
+        <v>4.04</v>
       </c>
       <c r="D68">
-        <v>165</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>43634</v>
+        <v>43653</v>
       </c>
       <c r="B69">
-        <v>14634</v>
+        <v>8642</v>
       </c>
       <c r="C69">
-        <v>11.06</v>
+        <v>6.53</v>
       </c>
       <c r="D69">
-        <v>498</v>
+        <v>294</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>43635</v>
+        <v>43654</v>
       </c>
       <c r="B70">
-        <v>8074</v>
+        <v>6611</v>
       </c>
       <c r="C70">
-        <v>6.1</v>
+        <v>5</v>
       </c>
       <c r="D70">
-        <v>383</v>
+        <v>225</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>43636</v>
+        <v>43655</v>
       </c>
       <c r="B71">
-        <v>5392</v>
+        <v>5872</v>
       </c>
       <c r="C71">
-        <v>4.08</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="D71">
-        <v>183</v>
+        <v>200</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>43637</v>
+        <v>43656</v>
       </c>
       <c r="B72">
-        <v>13215</v>
+        <v>5024</v>
       </c>
       <c r="C72">
-        <v>9.9</v>
+        <v>3.8</v>
       </c>
       <c r="D72">
-        <v>585</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>43638</v>
+        <v>43657</v>
       </c>
       <c r="B73">
-        <v>4571</v>
+        <v>12991</v>
       </c>
       <c r="C73">
-        <v>3.46</v>
+        <v>9.82</v>
       </c>
       <c r="D73">
-        <v>155</v>
+        <v>442</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>43639</v>
+        <v>43658</v>
       </c>
       <c r="B74">
-        <v>481</v>
+        <v>11051</v>
       </c>
       <c r="C74">
-        <v>0.36</v>
+        <v>8.35</v>
       </c>
       <c r="D74">
-        <v>16</v>
+        <v>376</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>43640</v>
+        <v>43659</v>
       </c>
       <c r="B75">
-        <v>6663</v>
+        <v>8858</v>
       </c>
       <c r="C75">
-        <v>5.04</v>
+        <v>6.7</v>
       </c>
       <c r="D75">
-        <v>367</v>
+        <v>301</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>43641</v>
+        <v>43660</v>
       </c>
       <c r="B76">
-        <v>4203</v>
+        <v>9145</v>
       </c>
       <c r="C76">
-        <v>3.18</v>
+        <v>6.91</v>
       </c>
       <c r="D76">
-        <v>143</v>
+        <v>428</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>43642</v>
+        <v>43661</v>
       </c>
       <c r="B77">
-        <v>10404</v>
+        <v>12197</v>
       </c>
       <c r="C77">
-        <v>7.87</v>
+        <v>9.2200000000000006</v>
       </c>
       <c r="D77">
-        <v>355</v>
+        <v>415</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>43643</v>
+        <v>43662</v>
       </c>
       <c r="B78">
-        <v>12662</v>
+        <v>3612</v>
       </c>
       <c r="C78">
-        <v>9.57</v>
+        <v>2.73</v>
       </c>
       <c r="D78">
-        <v>431</v>
+        <v>123</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>43644</v>
+        <v>43663</v>
       </c>
       <c r="B79">
-        <v>7332</v>
+        <v>3658</v>
       </c>
       <c r="C79">
-        <v>5.54</v>
+        <v>2.77</v>
       </c>
       <c r="D79">
-        <v>249</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>43645</v>
+        <v>43664</v>
       </c>
       <c r="B80">
-        <v>6122</v>
+        <v>15427</v>
       </c>
       <c r="C80">
-        <v>4.63</v>
+        <v>11.66</v>
       </c>
       <c r="D80">
-        <v>208</v>
+        <v>525</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>43646</v>
+        <v>43665</v>
       </c>
       <c r="B81">
-        <v>6625</v>
+        <v>9016</v>
       </c>
       <c r="C81">
-        <v>5.01</v>
+        <v>6.82</v>
       </c>
       <c r="D81">
-        <v>225</v>
+        <v>415</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>43647</v>
+        <v>43666</v>
       </c>
       <c r="B82">
-        <v>2296</v>
+        <v>3879</v>
       </c>
       <c r="C82">
-        <v>1.74</v>
+        <v>2.93</v>
       </c>
       <c r="D82">
-        <v>78</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>43648</v>
+        <v>43667</v>
       </c>
       <c r="B83">
-        <v>5171</v>
+        <v>10852</v>
       </c>
       <c r="C83">
-        <v>3.91</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D83">
-        <v>176</v>
+        <v>508</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>43649</v>
+        <v>43668</v>
       </c>
       <c r="B84">
-        <v>11882</v>
+        <v>3897</v>
       </c>
       <c r="C84">
-        <v>8.98</v>
+        <v>2.95</v>
       </c>
       <c r="D84">
-        <v>404</v>
+        <v>133</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>43650</v>
+        <v>43669</v>
       </c>
       <c r="B85">
-        <v>6006</v>
+        <v>4170</v>
       </c>
       <c r="C85">
-        <v>4.54</v>
+        <v>3.15</v>
       </c>
       <c r="D85">
-        <v>204</v>
+        <v>142</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>43651</v>
+        <v>43670</v>
       </c>
       <c r="B86">
-        <v>5774</v>
+        <v>2808</v>
       </c>
       <c r="C86">
-        <v>4.37</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D86">
-        <v>196</v>
+        <v>128</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>43652</v>
+        <v>43671</v>
       </c>
       <c r="B87">
-        <v>5344</v>
+        <v>5929</v>
       </c>
       <c r="C87">
-        <v>4.04</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="D87">
-        <v>182</v>
+        <v>202</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>43653</v>
+        <v>43672</v>
       </c>
       <c r="B88">
-        <v>8642</v>
+        <v>17624</v>
       </c>
       <c r="C88">
-        <v>6.53</v>
+        <v>13.32</v>
       </c>
       <c r="D88">
-        <v>294</v>
+        <v>600</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>43654</v>
+        <v>43673</v>
       </c>
       <c r="B89">
-        <v>6611</v>
+        <v>6040</v>
       </c>
       <c r="C89">
-        <v>5</v>
+        <v>4.57</v>
       </c>
       <c r="D89">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>43655</v>
+        <v>43674</v>
       </c>
       <c r="B90">
-        <v>5872</v>
+        <v>4057</v>
       </c>
       <c r="C90">
-        <v>4.4400000000000004</v>
+        <v>3.07</v>
       </c>
       <c r="D90">
-        <v>200</v>
+        <v>138</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>43656</v>
+        <v>43675</v>
       </c>
       <c r="B91">
-        <v>5024</v>
+        <v>9343</v>
       </c>
       <c r="C91">
-        <v>3.8</v>
+        <v>7.06</v>
       </c>
       <c r="D91">
-        <v>171</v>
+        <v>433</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>43657</v>
+        <v>43676</v>
       </c>
       <c r="B92">
-        <v>12991</v>
+        <v>8160</v>
       </c>
       <c r="C92">
-        <v>9.82</v>
+        <v>6.17</v>
       </c>
       <c r="D92">
-        <v>442</v>
+        <v>278</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>43658</v>
+        <v>43677</v>
       </c>
       <c r="B93">
-        <v>11051</v>
+        <v>3796</v>
       </c>
       <c r="C93">
-        <v>8.35</v>
+        <v>2.87</v>
       </c>
       <c r="D93">
-        <v>376</v>
+        <v>129</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>43659</v>
+        <v>43678</v>
       </c>
       <c r="B94">
-        <v>8858</v>
+        <v>6617</v>
       </c>
       <c r="C94">
-        <v>6.7</v>
+        <v>5</v>
       </c>
       <c r="D94">
-        <v>301</v>
+        <v>225</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>43660</v>
+        <v>43679</v>
       </c>
       <c r="B95">
-        <v>9145</v>
+        <v>7750</v>
       </c>
       <c r="C95">
-        <v>6.91</v>
+        <v>5.86</v>
       </c>
       <c r="D95">
-        <v>428</v>
+        <v>264</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>43661</v>
+        <v>43680</v>
       </c>
       <c r="B96">
-        <v>12197</v>
+        <v>7636</v>
       </c>
       <c r="C96">
-        <v>9.2200000000000006</v>
+        <v>5.77</v>
       </c>
       <c r="D96">
-        <v>415</v>
+        <v>260</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>43662</v>
+        <v>43681</v>
       </c>
       <c r="B97">
-        <v>3612</v>
+        <v>4074</v>
       </c>
       <c r="C97">
-        <v>2.73</v>
+        <v>3.08</v>
       </c>
       <c r="D97">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>43663</v>
+        <v>43682</v>
       </c>
       <c r="B98">
-        <v>3658</v>
+        <v>3310</v>
       </c>
       <c r="C98">
-        <v>2.77</v>
+        <v>2.5</v>
       </c>
       <c r="D98">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>43664</v>
+        <v>43683</v>
       </c>
       <c r="B99">
-        <v>15427</v>
+        <v>6527</v>
       </c>
       <c r="C99">
-        <v>11.66</v>
+        <v>4.93</v>
       </c>
       <c r="D99">
-        <v>525</v>
+        <v>222</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>43665</v>
+        <v>43684</v>
       </c>
       <c r="B100">
-        <v>9016</v>
+        <v>3653</v>
       </c>
       <c r="C100">
-        <v>6.82</v>
+        <v>2.76</v>
       </c>
       <c r="D100">
-        <v>415</v>
+        <v>124</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>43666</v>
+        <v>43685</v>
       </c>
       <c r="B101">
-        <v>3879</v>
+        <v>5937</v>
       </c>
       <c r="C101">
-        <v>2.93</v>
+        <v>4.49</v>
       </c>
       <c r="D101">
-        <v>132</v>
+        <v>202</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>43667</v>
+        <v>43686</v>
       </c>
       <c r="B102">
-        <v>10852</v>
+        <v>6192</v>
       </c>
       <c r="C102">
-        <v>8.1999999999999993</v>
+        <v>4.68</v>
       </c>
       <c r="D102">
-        <v>508</v>
+        <v>212</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>43668</v>
+        <v>43687</v>
       </c>
       <c r="B103">
-        <v>3897</v>
+        <v>7753</v>
       </c>
       <c r="C103">
-        <v>2.95</v>
+        <v>5.86</v>
       </c>
       <c r="D103">
-        <v>133</v>
+        <v>264</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>43669</v>
+        <v>43688</v>
       </c>
       <c r="B104">
-        <v>4170</v>
+        <v>8908</v>
       </c>
       <c r="C104">
-        <v>3.15</v>
+        <v>6.73</v>
       </c>
       <c r="D104">
-        <v>142</v>
+        <v>432</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>43670</v>
+        <v>43689</v>
       </c>
       <c r="B105">
-        <v>2808</v>
+        <v>5397</v>
       </c>
       <c r="C105">
-        <v>2.2000000000000002</v>
+        <v>4.08</v>
       </c>
       <c r="D105">
-        <v>128</v>
+        <v>184</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>43671</v>
+        <v>43690</v>
       </c>
       <c r="B106">
-        <v>5929</v>
+        <v>8336</v>
       </c>
       <c r="C106">
-        <v>4.4800000000000004</v>
+        <v>6.3</v>
       </c>
       <c r="D106">
-        <v>202</v>
+        <v>284</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>43672</v>
+        <v>43691</v>
       </c>
       <c r="B107">
-        <v>17624</v>
+        <v>4152</v>
       </c>
       <c r="C107">
-        <v>13.32</v>
+        <v>3.14</v>
       </c>
       <c r="D107">
-        <v>600</v>
+        <v>142</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>43673</v>
+        <v>43692</v>
       </c>
       <c r="B108">
-        <v>6040</v>
+        <v>10975</v>
       </c>
       <c r="C108">
-        <v>4.57</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="D108">
-        <v>205</v>
+        <v>373</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>43674</v>
+        <v>43693</v>
       </c>
       <c r="B109">
-        <v>4057</v>
+        <v>20005</v>
       </c>
       <c r="C109">
-        <v>3.07</v>
+        <v>15.12</v>
       </c>
       <c r="D109">
-        <v>138</v>
+        <v>870</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>43675</v>
+        <v>43694</v>
       </c>
       <c r="B110">
-        <v>9343</v>
+        <v>4778</v>
       </c>
       <c r="C110">
-        <v>7.06</v>
+        <v>3.61</v>
       </c>
       <c r="D110">
-        <v>433</v>
+        <v>163</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>43676</v>
+        <v>43695</v>
       </c>
       <c r="B111">
-        <v>8160</v>
+        <v>5256</v>
       </c>
       <c r="C111">
-        <v>6.17</v>
+        <v>3.97</v>
       </c>
       <c r="D111">
-        <v>278</v>
+        <v>179</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>43677</v>
+        <v>43696</v>
       </c>
       <c r="B112">
-        <v>3796</v>
+        <v>8341</v>
       </c>
       <c r="C112">
-        <v>2.87</v>
+        <v>6.31</v>
       </c>
       <c r="D112">
-        <v>129</v>
+        <v>284</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>43678</v>
+        <v>43697</v>
       </c>
       <c r="B113">
-        <v>6617</v>
+        <v>6055</v>
       </c>
       <c r="C113">
-        <v>5</v>
+        <v>4.58</v>
       </c>
       <c r="D113">
-        <v>225</v>
+        <v>206</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>43679</v>
+        <v>43698</v>
       </c>
       <c r="B114">
-        <v>7750</v>
+        <v>4204</v>
       </c>
       <c r="C114">
-        <v>5.86</v>
+        <v>3.18</v>
       </c>
       <c r="D114">
-        <v>264</v>
+        <v>143</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>43680</v>
+        <v>43699</v>
       </c>
       <c r="B115">
-        <v>7636</v>
+        <v>5216</v>
       </c>
       <c r="C115">
-        <v>5.77</v>
+        <v>3.94</v>
       </c>
       <c r="D115">
-        <v>260</v>
+        <v>177</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>43681</v>
+        <v>43700</v>
       </c>
       <c r="B116">
-        <v>4074</v>
+        <v>3080</v>
       </c>
       <c r="C116">
-        <v>3.08</v>
+        <v>2.33</v>
       </c>
       <c r="D116">
-        <v>139</v>
+        <v>105</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>43682</v>
+        <v>43701</v>
       </c>
       <c r="B117">
-        <v>3310</v>
+        <v>4737</v>
       </c>
       <c r="C117">
-        <v>2.5</v>
+        <v>3.58</v>
       </c>
       <c r="D117">
-        <v>113</v>
+        <v>161</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>43683</v>
+        <v>43702</v>
       </c>
       <c r="B118">
-        <v>6527</v>
+        <v>8109</v>
       </c>
       <c r="C118">
-        <v>4.93</v>
+        <v>6.13</v>
       </c>
       <c r="D118">
-        <v>222</v>
+        <v>276</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>43684</v>
+        <v>43703</v>
       </c>
       <c r="B119">
-        <v>3653</v>
+        <v>5530</v>
       </c>
       <c r="C119">
-        <v>2.76</v>
+        <v>4.18</v>
       </c>
       <c r="D119">
-        <v>124</v>
+        <v>188</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>43685</v>
+        <v>43704</v>
       </c>
       <c r="B120">
-        <v>5937</v>
+        <v>7716</v>
       </c>
       <c r="C120">
-        <v>4.49</v>
+        <v>5.83</v>
       </c>
       <c r="D120">
-        <v>202</v>
+        <v>264</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>43686</v>
+        <v>43705</v>
       </c>
       <c r="B121">
-        <v>6192</v>
+        <v>4535</v>
       </c>
       <c r="C121">
-        <v>4.68</v>
+        <v>3.43</v>
       </c>
       <c r="D121">
-        <v>212</v>
+        <v>154</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>43687</v>
+        <v>43706</v>
       </c>
       <c r="B122">
-        <v>7753</v>
+        <v>13863</v>
       </c>
       <c r="C122">
-        <v>5.86</v>
+        <v>10.48</v>
       </c>
       <c r="D122">
-        <v>264</v>
+        <v>472</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>43688</v>
+        <v>43707</v>
       </c>
       <c r="B123">
-        <v>8908</v>
+        <v>8111</v>
       </c>
       <c r="C123">
-        <v>6.73</v>
+        <v>6.13</v>
       </c>
       <c r="D123">
-        <v>432</v>
+        <v>276</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>43689</v>
+        <v>43708</v>
       </c>
       <c r="B124">
-        <v>5397</v>
+        <v>2039</v>
       </c>
       <c r="C124">
-        <v>4.08</v>
+        <v>1.54</v>
       </c>
       <c r="D124">
-        <v>184</v>
+        <v>69</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>43690</v>
+        <v>43709</v>
       </c>
       <c r="B125">
-        <v>8336</v>
+        <v>11462</v>
       </c>
       <c r="C125">
-        <v>6.3</v>
+        <v>8.66</v>
       </c>
       <c r="D125">
-        <v>284</v>
+        <v>492</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>43691</v>
+        <v>43710</v>
       </c>
       <c r="B126">
-        <v>4152</v>
+        <v>5376</v>
       </c>
       <c r="C126">
-        <v>3.14</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="D126">
-        <v>142</v>
+        <v>183</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>43692</v>
+        <v>43711</v>
       </c>
       <c r="B127">
-        <v>10975</v>
+        <v>8037</v>
       </c>
       <c r="C127">
-        <v>8.3000000000000007</v>
+        <v>6.08</v>
       </c>
       <c r="D127">
-        <v>373</v>
+        <v>275</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>43693</v>
+        <v>43712</v>
       </c>
       <c r="B128">
-        <v>20005</v>
+        <v>14488</v>
       </c>
       <c r="C128">
-        <v>15.12</v>
+        <v>10.95</v>
       </c>
       <c r="D128">
-        <v>870</v>
+        <v>493</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>43694</v>
+        <v>43713</v>
       </c>
       <c r="B129">
-        <v>4778</v>
+        <v>10788</v>
       </c>
       <c r="C129">
-        <v>3.61</v>
+        <v>8.15</v>
       </c>
       <c r="D129">
-        <v>163</v>
+        <v>367</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>43695</v>
+        <v>43714</v>
       </c>
       <c r="B130">
-        <v>5256</v>
+        <v>10515</v>
       </c>
       <c r="C130">
-        <v>3.97</v>
+        <v>7.93</v>
       </c>
       <c r="D130">
-        <v>179</v>
+        <v>358</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>43696</v>
+        <v>43715</v>
       </c>
       <c r="B131">
-        <v>8341</v>
+        <v>1084</v>
       </c>
       <c r="C131">
-        <v>6.31</v>
+        <v>0.82</v>
       </c>
       <c r="D131">
-        <v>284</v>
+        <v>37</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>43697</v>
+        <v>43716</v>
       </c>
       <c r="B132">
-        <v>6055</v>
+        <v>14803</v>
       </c>
       <c r="C132">
-        <v>4.58</v>
+        <v>11.19</v>
       </c>
       <c r="D132">
-        <v>206</v>
+        <v>637</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>43698</v>
+        <v>43717</v>
       </c>
       <c r="B133">
-        <v>4204</v>
+        <v>9047</v>
       </c>
       <c r="C133">
-        <v>3.18</v>
+        <v>6.84</v>
       </c>
       <c r="D133">
-        <v>143</v>
+        <v>308</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>43699</v>
+        <v>43718</v>
       </c>
       <c r="B134">
-        <v>5216</v>
+        <v>9175</v>
       </c>
       <c r="C134">
-        <v>3.94</v>
+        <v>6.94</v>
       </c>
       <c r="D134">
-        <v>177</v>
+        <v>312</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>43700</v>
+        <v>43719</v>
       </c>
       <c r="B135">
-        <v>3080</v>
+        <v>6975</v>
       </c>
       <c r="C135">
-        <v>2.33</v>
+        <v>5.27</v>
       </c>
       <c r="D135">
-        <v>105</v>
+        <v>237</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>43701</v>
+        <v>43720</v>
       </c>
       <c r="B136">
-        <v>4737</v>
+        <v>2674</v>
       </c>
       <c r="C136">
-        <v>3.58</v>
+        <v>2.02</v>
       </c>
       <c r="D136">
-        <v>161</v>
+        <v>91</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>43702</v>
+        <v>43721</v>
       </c>
       <c r="B137">
-        <v>8109</v>
+        <v>4197</v>
       </c>
       <c r="C137">
-        <v>6.13</v>
+        <v>3.17</v>
       </c>
       <c r="D137">
-        <v>276</v>
+        <v>143</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>43703</v>
+        <v>43722</v>
       </c>
       <c r="B138">
-        <v>5530</v>
+        <v>2952</v>
       </c>
       <c r="C138">
-        <v>4.18</v>
+        <v>2.23</v>
       </c>
       <c r="D138">
-        <v>188</v>
+        <v>100</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>43704</v>
+        <v>43723</v>
       </c>
       <c r="B139">
-        <v>7716</v>
+        <v>6476</v>
       </c>
       <c r="C139">
-        <v>5.83</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D139">
-        <v>264</v>
+        <v>220</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>43705</v>
+        <v>43724</v>
       </c>
       <c r="B140">
-        <v>4535</v>
+        <v>3885</v>
       </c>
       <c r="C140">
-        <v>3.43</v>
+        <v>2.94</v>
       </c>
       <c r="D140">
-        <v>154</v>
+        <v>132</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>43706</v>
+        <v>43725</v>
       </c>
       <c r="B141">
-        <v>13863</v>
+        <v>3471</v>
       </c>
       <c r="C141">
-        <v>10.48</v>
+        <v>2.62</v>
       </c>
       <c r="D141">
-        <v>472</v>
+        <v>118</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>43707</v>
+        <v>43726</v>
       </c>
       <c r="B142">
-        <v>8111</v>
+        <v>1608</v>
       </c>
       <c r="C142">
-        <v>6.13</v>
+        <v>1.22</v>
       </c>
       <c r="D142">
-        <v>276</v>
+        <v>55</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>43708</v>
+        <v>43727</v>
       </c>
       <c r="B143">
-        <v>2039</v>
+        <v>4349</v>
       </c>
       <c r="C143">
-        <v>1.54</v>
+        <v>3.29</v>
       </c>
       <c r="D143">
-        <v>69</v>
+        <v>148</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>43709</v>
+        <v>43728</v>
       </c>
       <c r="B144">
-        <v>11462</v>
+        <v>4884</v>
       </c>
       <c r="C144">
-        <v>8.66</v>
+        <v>3.69</v>
       </c>
       <c r="D144">
-        <v>492</v>
+        <v>166</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>43710</v>
+        <v>43729</v>
       </c>
       <c r="B145">
-        <v>5376</v>
+        <v>202</v>
       </c>
       <c r="C145">
-        <v>4.0599999999999996</v>
+        <v>0.15</v>
       </c>
       <c r="D145">
-        <v>183</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>43711</v>
+        <v>43730</v>
       </c>
       <c r="B146">
-        <v>8037</v>
+        <v>3870</v>
       </c>
       <c r="C146">
-        <v>6.08</v>
+        <v>2.93</v>
       </c>
       <c r="D146">
-        <v>275</v>
+        <v>132</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>43712</v>
+        <v>43731</v>
       </c>
       <c r="B147">
-        <v>14488</v>
+        <v>7714</v>
       </c>
       <c r="C147">
-        <v>10.95</v>
+        <v>5.83</v>
       </c>
       <c r="D147">
-        <v>493</v>
+        <v>262</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>43713</v>
+        <v>43732</v>
       </c>
       <c r="B148">
-        <v>10788</v>
+        <v>7711</v>
       </c>
       <c r="C148">
-        <v>8.15</v>
+        <v>5.83</v>
       </c>
       <c r="D148">
-        <v>367</v>
+        <v>262</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>43714</v>
+        <v>43733</v>
       </c>
       <c r="B149">
-        <v>10515</v>
+        <v>4778</v>
       </c>
       <c r="C149">
-        <v>7.93</v>
+        <v>3.61</v>
       </c>
       <c r="D149">
-        <v>358</v>
+        <v>163</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>43715</v>
+        <v>43734</v>
       </c>
       <c r="B150">
-        <v>1084</v>
+        <v>10523</v>
       </c>
       <c r="C150">
-        <v>0.82</v>
+        <v>7.96</v>
       </c>
       <c r="D150">
-        <v>37</v>
+        <v>358</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>43716</v>
+        <v>43735</v>
       </c>
       <c r="B151">
-        <v>14803</v>
+        <v>4859</v>
       </c>
       <c r="C151">
-        <v>11.19</v>
+        <v>3.67</v>
       </c>
       <c r="D151">
-        <v>637</v>
+        <v>165</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>43717</v>
+        <v>43736</v>
       </c>
       <c r="B152">
-        <v>9047</v>
+        <v>6552</v>
       </c>
       <c r="C152">
-        <v>6.84</v>
+        <v>4.95</v>
       </c>
       <c r="D152">
-        <v>308</v>
+        <v>325</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>43718</v>
+        <v>43737</v>
       </c>
       <c r="B153">
-        <v>9175</v>
+        <v>33058</v>
       </c>
       <c r="C153">
-        <v>6.94</v>
+        <v>24.99</v>
       </c>
       <c r="D153">
-        <v>312</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>43719</v>
+        <v>43738</v>
       </c>
       <c r="B154">
-        <v>6975</v>
+        <v>16693</v>
       </c>
       <c r="C154">
-        <v>5.27</v>
+        <v>12.62</v>
       </c>
       <c r="D154">
-        <v>237</v>
+        <v>568</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>43720</v>
+        <v>43739</v>
       </c>
       <c r="B155">
-        <v>2674</v>
+        <v>17007</v>
       </c>
       <c r="C155">
-        <v>2.02</v>
+        <v>12.86</v>
       </c>
       <c r="D155">
-        <v>91</v>
+        <v>579</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>43721</v>
+        <v>43740</v>
       </c>
       <c r="B156">
-        <v>4197</v>
+        <v>6629</v>
       </c>
       <c r="C156">
-        <v>3.17</v>
+        <v>5.01</v>
       </c>
       <c r="D156">
-        <v>143</v>
+        <v>225</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>43722</v>
+        <v>43741</v>
       </c>
       <c r="B157">
-        <v>2952</v>
+        <v>10044</v>
       </c>
       <c r="C157">
-        <v>2.23</v>
+        <v>7.59</v>
       </c>
       <c r="D157">
-        <v>100</v>
+        <v>342</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>43723</v>
+        <v>43742</v>
       </c>
       <c r="B158">
-        <v>6476</v>
+        <v>8935</v>
       </c>
       <c r="C158">
-        <v>4.9000000000000004</v>
+        <v>6.75</v>
       </c>
       <c r="D158">
-        <v>220</v>
+        <v>304</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>43724</v>
+        <v>43743</v>
       </c>
       <c r="B159">
-        <v>3885</v>
+        <v>18795</v>
       </c>
       <c r="C159">
-        <v>2.94</v>
+        <v>14.21</v>
       </c>
       <c r="D159">
-        <v>132</v>
+        <v>639</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>43725</v>
+        <v>43744</v>
       </c>
       <c r="B160">
-        <v>3471</v>
+        <v>15448</v>
       </c>
       <c r="C160">
-        <v>2.62</v>
+        <v>11.68</v>
       </c>
       <c r="D160">
-        <v>118</v>
+        <v>526</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>43726</v>
+        <v>43745</v>
       </c>
       <c r="B161">
-        <v>1608</v>
+        <v>4030</v>
       </c>
       <c r="C161">
-        <v>1.22</v>
+        <v>3.05</v>
       </c>
       <c r="D161">
-        <v>55</v>
+        <v>137</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>43727</v>
+        <v>43746</v>
       </c>
       <c r="B162">
-        <v>4349</v>
+        <v>4202</v>
       </c>
       <c r="C162">
-        <v>3.29</v>
+        <v>3.18</v>
       </c>
       <c r="D162">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>43728</v>
+        <v>43747</v>
       </c>
       <c r="B163">
-        <v>4884</v>
+        <v>6677</v>
       </c>
       <c r="C163">
-        <v>3.69</v>
+        <v>5.05</v>
       </c>
       <c r="D163">
-        <v>166</v>
+        <v>227</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>43729</v>
+        <v>43748</v>
       </c>
       <c r="B164">
-        <v>202</v>
+        <v>8237</v>
       </c>
       <c r="C164">
-        <v>0.15</v>
+        <v>6.23</v>
       </c>
       <c r="D164">
-        <v>7</v>
+        <v>280</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>43730</v>
+        <v>43749</v>
       </c>
       <c r="B165">
-        <v>3870</v>
+        <v>5086</v>
       </c>
       <c r="C165">
-        <v>2.93</v>
+        <v>3.85</v>
       </c>
       <c r="D165">
-        <v>132</v>
+        <v>173</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>43731</v>
+        <v>43750</v>
       </c>
       <c r="B166">
-        <v>7714</v>
+        <v>341</v>
       </c>
       <c r="C166">
-        <v>5.83</v>
+        <v>0.26</v>
       </c>
       <c r="D166">
-        <v>262</v>
+        <v>12</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>43732</v>
+        <v>43751</v>
       </c>
       <c r="B167">
-        <v>7711</v>
+        <v>2210</v>
       </c>
       <c r="C167">
-        <v>5.83</v>
+        <v>1.67</v>
       </c>
       <c r="D167">
-        <v>262</v>
+        <v>75</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>43733</v>
+        <v>43752</v>
       </c>
       <c r="B168">
-        <v>4778</v>
+        <v>4723</v>
       </c>
       <c r="C168">
-        <v>3.61</v>
+        <v>3.57</v>
       </c>
       <c r="D168">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>43734</v>
+        <v>43753</v>
       </c>
       <c r="B169">
-        <v>10523</v>
+        <v>4284</v>
       </c>
       <c r="C169">
-        <v>7.96</v>
+        <v>3.24</v>
       </c>
       <c r="D169">
-        <v>358</v>
+        <v>146</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>43735</v>
+        <v>43754</v>
       </c>
       <c r="B170">
-        <v>4859</v>
+        <v>4424</v>
       </c>
       <c r="C170">
-        <v>3.67</v>
+        <v>3.34</v>
       </c>
       <c r="D170">
-        <v>165</v>
+        <v>150</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>43736</v>
+        <v>43755</v>
       </c>
       <c r="B171">
-        <v>6552</v>
+        <v>6573</v>
       </c>
       <c r="C171">
-        <v>4.95</v>
+        <v>4.97</v>
       </c>
       <c r="D171">
-        <v>325</v>
+        <v>224</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>43737</v>
+        <v>43756</v>
       </c>
       <c r="B172">
-        <v>33058</v>
+        <v>3908</v>
       </c>
       <c r="C172">
-        <v>24.99</v>
+        <v>2.95</v>
       </c>
       <c r="D172">
-        <v>1125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>43738</v>
+        <v>43757</v>
       </c>
       <c r="B173">
-        <v>16693</v>
+        <v>1822</v>
       </c>
       <c r="C173">
-        <v>12.62</v>
+        <v>1.38</v>
       </c>
       <c r="D173">
-        <v>568</v>
+        <v>62</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>43739</v>
+        <v>43758</v>
       </c>
       <c r="B174">
-        <v>17007</v>
+        <v>8086</v>
       </c>
       <c r="C174">
-        <v>12.86</v>
+        <v>6.11</v>
       </c>
       <c r="D174">
-        <v>579</v>
+        <v>275</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>43740</v>
+        <v>43759</v>
       </c>
       <c r="B175">
-        <v>6629</v>
+        <v>8130</v>
       </c>
       <c r="C175">
-        <v>5.01</v>
+        <v>6.15</v>
       </c>
       <c r="D175">
-        <v>225</v>
+        <v>277</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>43741</v>
+        <v>43760</v>
       </c>
       <c r="B176">
-        <v>10044</v>
+        <v>4530</v>
       </c>
       <c r="C176">
-        <v>7.59</v>
+        <v>3.42</v>
       </c>
       <c r="D176">
-        <v>342</v>
+        <v>154</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>43742</v>
+        <v>43761</v>
       </c>
       <c r="B177">
-        <v>8935</v>
+        <v>7078</v>
       </c>
       <c r="C177">
-        <v>6.75</v>
+        <v>5.35</v>
       </c>
       <c r="D177">
-        <v>304</v>
+        <v>245</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>43743</v>
+        <v>43762</v>
       </c>
       <c r="B178">
-        <v>18795</v>
+        <v>11525</v>
       </c>
       <c r="C178">
-        <v>14.21</v>
+        <v>8.7100000000000009</v>
       </c>
       <c r="D178">
-        <v>639</v>
+        <v>394</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>43744</v>
+        <v>43763</v>
       </c>
       <c r="B179">
-        <v>15448</v>
+        <v>2702</v>
       </c>
       <c r="C179">
-        <v>11.68</v>
+        <v>2.04</v>
       </c>
       <c r="D179">
-        <v>526</v>
+        <v>92</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>43745</v>
+        <v>43764</v>
       </c>
       <c r="B180">
-        <v>4030</v>
+        <v>3431</v>
       </c>
       <c r="C180">
-        <v>3.05</v>
+        <v>2.59</v>
       </c>
       <c r="D180">
-        <v>137</v>
+        <v>117</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
-        <v>43746</v>
+        <v>43765</v>
       </c>
       <c r="B181">
-        <v>4202</v>
+        <v>4400</v>
       </c>
       <c r="C181">
-        <v>3.18</v>
+        <v>3.33</v>
       </c>
       <c r="D181">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>43747</v>
+        <v>43766</v>
       </c>
       <c r="B182">
-        <v>6677</v>
+        <v>4140</v>
       </c>
       <c r="C182">
-        <v>5.05</v>
+        <v>3.13</v>
       </c>
       <c r="D182">
-        <v>227</v>
+        <v>144</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>43748</v>
+        <v>43767</v>
       </c>
       <c r="B183">
-        <v>8237</v>
+        <v>4236</v>
       </c>
       <c r="C183">
-        <v>6.23</v>
+        <v>3.2</v>
       </c>
       <c r="D183">
-        <v>280</v>
+        <v>144</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>43749</v>
+        <v>43768</v>
       </c>
       <c r="B184">
-        <v>5086</v>
+        <v>9132</v>
       </c>
       <c r="C184">
-        <v>3.85</v>
+        <v>6.9</v>
       </c>
       <c r="D184">
-        <v>173</v>
+        <v>311</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>43750</v>
+        <v>43769</v>
       </c>
       <c r="B185">
-        <v>341</v>
+        <v>5766</v>
       </c>
       <c r="C185">
-        <v>0.26</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="D185">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="1">
-        <v>43751</v>
-      </c>
-      <c r="B186">
-        <v>2210</v>
-      </c>
-      <c r="C186">
-        <v>1.67</v>
-      </c>
-      <c r="D186">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="1">
-        <v>43752</v>
-      </c>
-      <c r="B187">
-        <v>4723</v>
-      </c>
-      <c r="C187">
-        <v>3.57</v>
-      </c>
-      <c r="D187">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="1">
-        <v>43753</v>
-      </c>
-      <c r="B188">
-        <v>4284</v>
-      </c>
-      <c r="C188">
-        <v>3.24</v>
-      </c>
-      <c r="D188">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="1">
-        <v>43754</v>
-      </c>
-      <c r="B189">
-        <v>4424</v>
-      </c>
-      <c r="C189">
-        <v>3.34</v>
-      </c>
-      <c r="D189">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="1">
-        <v>43755</v>
-      </c>
-      <c r="B190">
-        <v>6573</v>
-      </c>
-      <c r="C190">
-        <v>4.97</v>
-      </c>
-      <c r="D190">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="1">
-        <v>43756</v>
-      </c>
-      <c r="B191">
-        <v>3908</v>
-      </c>
-      <c r="C191">
-        <v>2.95</v>
-      </c>
-      <c r="D191">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="1">
-        <v>43757</v>
-      </c>
-      <c r="B192">
-        <v>1822</v>
-      </c>
-      <c r="C192">
-        <v>1.38</v>
-      </c>
-      <c r="D192">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="1">
-        <v>43758</v>
-      </c>
-      <c r="B193">
-        <v>8086</v>
-      </c>
-      <c r="C193">
-        <v>6.11</v>
-      </c>
-      <c r="D193">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="1">
-        <v>43759</v>
-      </c>
-      <c r="B194">
-        <v>8130</v>
-      </c>
-      <c r="C194">
-        <v>6.15</v>
-      </c>
-      <c r="D194">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="1">
-        <v>43760</v>
-      </c>
-      <c r="B195">
-        <v>4530</v>
-      </c>
-      <c r="C195">
-        <v>3.42</v>
-      </c>
-      <c r="D195">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="1">
-        <v>43761</v>
-      </c>
-      <c r="B196">
-        <v>7078</v>
-      </c>
-      <c r="C196">
-        <v>5.35</v>
-      </c>
-      <c r="D196">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="1">
-        <v>43762</v>
-      </c>
-      <c r="B197">
-        <v>11525</v>
-      </c>
-      <c r="C197">
-        <v>8.7100000000000009</v>
-      </c>
-      <c r="D197">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="1">
-        <v>43763</v>
-      </c>
-      <c r="B198">
-        <v>2702</v>
-      </c>
-      <c r="C198">
-        <v>2.04</v>
-      </c>
-      <c r="D198">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="1">
-        <v>43764</v>
-      </c>
-      <c r="B199">
-        <v>3431</v>
-      </c>
-      <c r="C199">
-        <v>2.59</v>
-      </c>
-      <c r="D199">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="1">
-        <v>43765</v>
-      </c>
-      <c r="B200">
-        <v>4400</v>
-      </c>
-      <c r="C200">
-        <v>3.33</v>
-      </c>
-      <c r="D200">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="1">
-        <v>43766</v>
-      </c>
-      <c r="B201">
-        <v>4140</v>
-      </c>
-      <c r="C201">
-        <v>3.13</v>
-      </c>
-      <c r="D201">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="1">
-        <v>43767</v>
-      </c>
-      <c r="B202">
-        <v>4236</v>
-      </c>
-      <c r="C202">
-        <v>3.2</v>
-      </c>
-      <c r="D202">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="1">
-        <v>43768</v>
-      </c>
-      <c r="B203">
-        <v>9132</v>
-      </c>
-      <c r="C203">
-        <v>6.9</v>
-      </c>
-      <c r="D203">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="1">
-        <v>43769</v>
-      </c>
-      <c r="B204">
-        <v>5766</v>
-      </c>
-      <c r="C204">
-        <v>4.3600000000000003</v>
-      </c>
-      <c r="D204">
         <v>196</v>
       </c>
     </row>

</xml_diff>